<commit_message>
Update to latest FPGA pof file
</commit_message>
<xml_diff>
--- a/Kicad/ElectronULA - MAX 10 Board V1.05/BOM.xlsx
+++ b/Kicad/ElectronULA - MAX 10 Board V1.05/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kicad - Electron ULA\ElectronULA - MAX 10 Board V1.05 with data buffer resistors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ElectronULA\Kicad\ElectronULA - MAX 10 Board V1.05\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -345,13 +345,13 @@
     <t>R32, R33, R34, R35, R36, R37, R38, R39</t>
   </si>
   <si>
-    <t>300 Ohm Resistor</t>
-  </si>
-  <si>
     <t>Slow down Data Buffers to reduce noise</t>
   </si>
   <si>
     <t>C1, C2, C3, C4, C5, C6, C7, C8, C9, C10, C11, C12, C13, C14, C15, C16, C17, C18, C19, C21, C22, C23, C24, C26, C28, C30, C31</t>
+  </si>
+  <si>
+    <t>33 Ohm Resistor</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1094,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>19</v>
@@ -1403,10 +1403,10 @@
         <v>8</v>
       </c>
       <c r="E36" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="G36" s="16"/>
     </row>

</xml_diff>